<commit_message>
Start with uncertainties.py, random values for environmental config work, animal config still doesn't add any new values.
life_cycle_assessment.py: Making the Show/Hide buttons work again
</commit_message>
<xml_diff>
--- a/default_configs/default_environmental_config.xlsx
+++ b/default_configs/default_environmental_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achermann\Project ReFuel\LCA tool developement\Manure Tool\default_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E22526-4131-4333-ACA0-72A46CA312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE851829-3150-43A4-8902-FA2B23BA21E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1223,7 +1223,9 @@
       <c r="B27" s="1">
         <v>0.5</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>0.05</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1236,7 +1238,9 @@
       <c r="B28" s="1">
         <v>0.4</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>0.04</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1249,7 +1253,9 @@
       <c r="B29" s="1">
         <v>0.85</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2">
+        <v>0.05</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1264,7 +1270,9 @@
       <c r="B30" s="1">
         <v>0.48</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>0.04</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
added montecrlo simulation, working on implementing PRCC and/or regression analysis
</commit_message>
<xml_diff>
--- a/default_configs/default_environmental_config.xlsx
+++ b/default_configs/default_environmental_config.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achermann\Project ReFuel\LCA tool developement\Manure Tool\default_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5088C-D53F-4EC1-BBDD-2F1E84F7928C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A81C1E6-0DD1-4308-AF97-2BC0CBD5BDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50988" yWindow="-1716" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -829,14 +828,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.7265625" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="84.7265625" customWidth="1"/>
   </cols>
@@ -1332,7 +1331,7 @@
         <v>0.5</v>
       </c>
       <c r="C31" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>5</v>
@@ -1347,7 +1346,7 @@
         <v>0.4</v>
       </c>
       <c r="C32" s="2">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
@@ -1362,7 +1361,7 @@
         <v>0.85</v>
       </c>
       <c r="C33" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
@@ -1379,7 +1378,7 @@
         <v>0.48</v>
       </c>
       <c r="C34" s="2">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>36</v>
@@ -1395,7 +1394,9 @@
       <c r="B35" s="1">
         <v>0.46700000000000003</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1410,7 +1411,9 @@
       <c r="B36" s="1">
         <v>0.51300000000000001</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1425,7 +1428,9 @@
       <c r="B37" s="1">
         <v>0.5</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1445,9 @@
       <c r="B38" s="1">
         <v>0.7</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1455,7 +1462,9 @@
       <c r="B39" s="1">
         <v>0.1</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>0.02</v>
+      </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1470,7 +1479,9 @@
       <c r="B40" s="1">
         <v>0.6</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1485,7 +1496,9 @@
       <c r="B41" s="1">
         <v>0.4</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="2">
+        <v>0.04</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1500,7 +1513,9 @@
       <c r="B42" s="1">
         <v>0.02</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2">
+        <v>2E-3</v>
+      </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1515,7 +1530,9 @@
       <c r="B43" s="1">
         <v>0.8</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D43" s="1" t="s">
         <v>5</v>
       </c>
@@ -1530,7 +1547,9 @@
       <c r="B44" s="1">
         <v>0.85</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2">
+        <v>0.02</v>
+      </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1545,7 +1564,9 @@
       <c r="B45" s="1">
         <v>0.9</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2">
+        <v>0.05</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1560,7 +1581,9 @@
       <c r="B46" s="1">
         <v>3500</v>
       </c>
-      <c r="C46" s="2"/>
+      <c r="C46" s="2">
+        <v>150</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>68</v>
       </c>
@@ -1648,7 +1671,9 @@
       <c r="B52" s="1">
         <v>5.5999999999999999E-5</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2">
+        <v>5.0000000000000004E-6</v>
+      </c>
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
@@ -1663,7 +1688,9 @@
       <c r="B53" s="1">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2">
+        <v>1E-4</v>
+      </c>
       <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1851,6 +1878,9 @@
       <c r="B66">
         <v>0.8</v>
       </c>
+      <c r="C66">
+        <v>0.01</v>
+      </c>
       <c r="D66" t="s">
         <v>5</v>
       </c>
@@ -1865,6 +1895,9 @@
       <c r="B67">
         <v>0.85</v>
       </c>
+      <c r="C67">
+        <v>0.01</v>
+      </c>
       <c r="D67" t="s">
         <v>5</v>
       </c>
@@ -1879,6 +1912,9 @@
       <c r="B68">
         <v>0.9</v>
       </c>
+      <c r="C68">
+        <v>0.01</v>
+      </c>
       <c r="D68" t="s">
         <v>5</v>
       </c>
@@ -1892,6 +1928,9 @@
       </c>
       <c r="B69">
         <v>0.7</v>
+      </c>
+      <c r="C69">
+        <v>0.04</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added framework for better uncertainty analysis to both env config and uncertainties.py
</commit_message>
<xml_diff>
--- a/default_configs/default_environmental_config.xlsx
+++ b/default_configs/default_environmental_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achermann\Project ReFuel\LCA tool developement\Manure Tool\default_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A81C1E6-0DD1-4308-AF97-2BC0CBD5BDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA522CC2-9C02-48E1-B063-4DAC8AED1D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50988" yWindow="-1716" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="1185" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="181">
   <si>
     <t>value</t>
   </si>
@@ -221,24 +221,6 @@
     <t>percentage of total CH4 produced, that is lost during AD process</t>
   </si>
   <si>
-    <t>ad_efficiency_small</t>
-  </si>
-  <si>
-    <t>ad_efficiency_medium</t>
-  </si>
-  <si>
-    <t>ad_efficiency_large</t>
-  </si>
-  <si>
-    <t>efficiency of AD plant in converting methane potential into methane gas for small plant</t>
-  </si>
-  <si>
-    <t>efficiency of AD plant in converting methane potential into methane gas for medium plant</t>
-  </si>
-  <si>
-    <t>efficiency of AD plant in converting methane potential into methane gas for large plant</t>
-  </si>
-  <si>
     <t>heat_demand_ad</t>
   </si>
   <si>
@@ -467,21 +449,12 @@
     <t>GWP 100 of AD plant construction according to Ecoinvent (lifetime 20 years for construction, 10 years for machinery)</t>
   </si>
   <si>
-    <t>generator production, mini CHP plant</t>
-  </si>
-  <si>
     <t>GWP 100 of heating with oil per MJ of energy, according to Ecoinvent</t>
   </si>
   <si>
-    <t>heat production, light fuel oil, at boiler 100kW, non-modulating</t>
-  </si>
-  <si>
     <t>GWP 100 of heating with natural gas per MJ of energy, according to Ecoinvent</t>
   </si>
   <si>
-    <t>heat production, natural gas, at boiler condensing modulating &lt;100kW</t>
-  </si>
-  <si>
     <t>co2_eq_oil_heating</t>
   </si>
   <si>
@@ -495,6 +468,117 @@
   </si>
   <si>
     <t>kg co2 / kWh</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Distribution function</t>
+  </si>
+  <si>
+    <t>Ecoinvent, heat production, natural gas, at boiler condensing modulating &lt;100kW, Region Switzerland</t>
+  </si>
+  <si>
+    <t>Ecoinvent, heat production, light fuel oil, at boiler 100kW, non-modulating, region Switzerland</t>
+  </si>
+  <si>
+    <t>Ecoinvent, region Switzerland</t>
+  </si>
+  <si>
+    <t>Ecoinvent, generator production, mini CHP plant, Region Switzerland</t>
+  </si>
+  <si>
+    <t>Method of Ecological Scarcity</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>lognormal</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Uniform or triangle</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>Holliger et al.</t>
+  </si>
+  <si>
+    <t>Webb et al.</t>
+  </si>
+  <si>
+    <t>Amon et al.</t>
+  </si>
+  <si>
+    <t>? Triangle</t>
+  </si>
+  <si>
+    <t>Ökostrom Stoffflussanalyse (Dinkel &amp; Kägi)</t>
+  </si>
+  <si>
+    <t>Wechselberg et al.</t>
+  </si>
+  <si>
+    <t>lognormal / triangle?</t>
+  </si>
+  <si>
+    <t>Krebs &amp; Frischknecht, 2021</t>
+  </si>
+  <si>
+    <t>Paine et al.</t>
+  </si>
+  <si>
+    <t>Ahring et al., Bruni et al. Li et al.</t>
+  </si>
+  <si>
+    <t>Makaruk et al.</t>
+  </si>
+  <si>
+    <t>Wang et al.</t>
+  </si>
+  <si>
+    <t>Ardolino et al.</t>
+  </si>
+  <si>
+    <t>IPCC 2021</t>
+  </si>
+  <si>
+    <t>Schnorf et al.</t>
+  </si>
+  <si>
+    <t>Liu et al.</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -510,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,12 +604,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +623,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,10 +915,12 @@
     <col min="1" max="1" width="40.7265625" customWidth="1"/>
     <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="84.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="15" max="15" width="23.08984375" customWidth="1"/>
+    <col min="16" max="16" width="84.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -854,10 +934,43 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" t="s">
+        <v>179</v>
+      </c>
+      <c r="O1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -871,10 +984,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -887,8 +1003,11 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -901,8 +1020,11 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -916,10 +1038,13 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="P5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -933,10 +1058,13 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
+        <v>155</v>
+      </c>
+      <c r="P6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -950,10 +1078,13 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="P7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -967,10 +1098,13 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
+        <v>155</v>
+      </c>
+      <c r="P8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -984,10 +1118,13 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="P9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1001,10 +1138,13 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
+        <v>155</v>
+      </c>
+      <c r="P10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1018,10 +1158,13 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
+        <v>155</v>
+      </c>
+      <c r="P11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1035,10 +1178,13 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
+        <v>155</v>
+      </c>
+      <c r="P12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1052,10 +1198,13 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
+        <v>155</v>
+      </c>
+      <c r="P13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1069,12 +1218,15 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
+        <v>155</v>
+      </c>
+      <c r="P14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B15">
         <f>B8/B11</f>
@@ -1083,26 +1235,35 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <f>B10/B13</f>
         <v>0.31818181818181818</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B17">
         <f>B10/B14</f>
         <v>0.82352941176470584</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1115,11 +1276,21 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18">
+        <f>B18</f>
+        <v>36</v>
+      </c>
+      <c r="O18" t="s">
+        <v>174</v>
+      </c>
+      <c r="P18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1132,11 +1303,21 @@
       <c r="D19" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H19">
+        <f>B19</f>
+        <v>298</v>
+      </c>
+      <c r="O19" t="s">
+        <v>174</v>
+      </c>
+      <c r="P19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1147,15 +1328,25 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20">
+        <f>B20</f>
+        <v>2.62</v>
+      </c>
+      <c r="O20" t="s">
+        <v>175</v>
+      </c>
+      <c r="P20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B21">
         <v>0.128</v>
@@ -1164,15 +1355,25 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H21">
+        <f>B21</f>
+        <v>0.128</v>
+      </c>
+      <c r="O21" t="s">
+        <v>168</v>
+      </c>
+      <c r="P21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B22">
         <v>0.26</v>
@@ -1181,83 +1382,124 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H22">
+        <f>B22</f>
+        <v>0.26</v>
+      </c>
+      <c r="O22" t="s">
+        <v>168</v>
+      </c>
+      <c r="P22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B23">
         <f>0.073405 / 3.6</f>
         <v>2.0390277777777778E-2</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H23">
+        <f>B23</f>
+        <v>2.0390277777777778E-2</v>
+      </c>
+      <c r="O23" t="s">
         <v>146</v>
       </c>
-      <c r="G23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="P23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B24">
         <f xml:space="preserve"> 0.10224 / 3.6</f>
         <v>2.8399999999999998E-2</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" t="s">
-        <v>144</v>
-      </c>
-      <c r="G24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H24">
+        <f>B24</f>
+        <v>2.8399999999999998E-2</v>
+      </c>
+      <c r="O24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B25">
         <f>3.6493* 10^4</f>
         <v>36493</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H25">
+        <f>B25</f>
+        <v>36493</v>
+      </c>
+      <c r="O25" t="s">
+        <v>148</v>
+      </c>
+      <c r="P25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B26">
         <v>61.816000000000003</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" t="s">
-        <v>141</v>
-      </c>
-      <c r="G26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26">
+        <f>B26</f>
+        <v>61.816000000000003</v>
+      </c>
+      <c r="O26" t="s">
+        <v>149</v>
+      </c>
+      <c r="P26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B27">
         <v>44000</v>
@@ -1266,15 +1508,25 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27">
+        <f>B27</f>
+        <v>44000</v>
+      </c>
+      <c r="O27" t="s">
+        <v>150</v>
+      </c>
+      <c r="P27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B28">
         <v>1000</v>
@@ -1283,15 +1535,25 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H28">
+        <f>B28</f>
+        <v>1000</v>
+      </c>
+      <c r="O28" t="s">
+        <v>150</v>
+      </c>
+      <c r="P28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B29">
         <v>8.3000000000000007</v>
@@ -1300,15 +1562,25 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29">
+        <f>B29</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="O29" t="s">
+        <v>150</v>
+      </c>
+      <c r="P29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B30">
         <v>2.8</v>
@@ -1317,627 +1589,1121 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30">
+        <f>B30</f>
+        <v>2.8</v>
+      </c>
+      <c r="O30" t="s">
+        <v>150</v>
+      </c>
+      <c r="P30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>0.5</v>
       </c>
       <c r="C31" s="2">
         <v>0.01</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H31" s="2">
+        <f>B31</f>
+        <v>0.5</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="O31" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>0.4</v>
       </c>
       <c r="C32" s="2">
         <v>0.01</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="H32" s="2">
+        <f>B32</f>
+        <v>0.4</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="O32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>0.85</v>
       </c>
       <c r="C33" s="2">
         <v>0.01</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H33" s="2">
+        <f>B33</f>
+        <v>0.85</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="O33" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P33" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>0.48</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>0.01</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" s="1">
+        <f>B34</f>
+        <v>0.48</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>0.46700000000000003</v>
       </c>
       <c r="C35" s="2">
         <v>0.01</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2">
+        <f>B35</f>
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="O35" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P35" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>0.51300000000000001</v>
       </c>
       <c r="C36" s="2">
         <v>0.01</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
+        <f>B36</f>
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="O36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>0.5</v>
       </c>
       <c r="C37" s="2">
         <v>0.01</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2">
+        <f>B37</f>
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="O37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>0.7</v>
       </c>
       <c r="C38" s="2">
         <v>0.01</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2">
+        <f>B38</f>
+        <v>0.7</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="O38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>0.1</v>
       </c>
       <c r="C39" s="2">
         <v>0.02</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2">
+        <f>B39</f>
+        <v>0.1</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="O39" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P39" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>0.6</v>
       </c>
       <c r="C40" s="2">
         <v>0.01</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2">
+        <f>B40</f>
+        <v>0.6</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>0.4</v>
       </c>
       <c r="C41" s="2">
         <v>0.04</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="D41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2">
+        <f>B41</f>
+        <v>0.4</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="1">
-        <v>0.02</v>
+      <c r="B42" s="2">
+        <v>1E-3</v>
       </c>
       <c r="C42" s="2">
         <v>2E-3</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="D42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H42" s="2">
+        <f>B42</f>
+        <v>1E-3</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="O42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
+        <v>3500</v>
+      </c>
+      <c r="C43" s="2">
+        <v>150</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2">
+        <f t="shared" ref="H43:H66" si="0">B43</f>
+        <v>3500</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="O43" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="O44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="O45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="2">
+        <v>3.5999999999999998E-6</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999998E-6</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="O46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="2">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="O47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="O48" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="2">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="O49" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="O50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" s="2">
+        <v>4</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="O51" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="O52" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="O53" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="O54" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D55" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" t="s">
+        <v>152</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56">
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>152</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57">
+        <v>1.72E-2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>152</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="0"/>
+        <v>1.72E-2</v>
+      </c>
+      <c r="O57" t="s">
+        <v>173</v>
+      </c>
+      <c r="P57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58">
+        <v>0.4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>152</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="O58" t="s">
+        <v>173</v>
+      </c>
+      <c r="P58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>152</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="O59" t="s">
+        <v>173</v>
+      </c>
+      <c r="P59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>152</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="O60" t="s">
+        <v>173</v>
+      </c>
+      <c r="P60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61">
+        <v>0.98939999999999995</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>152</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98939999999999995</v>
+      </c>
+      <c r="O61" t="s">
+        <v>173</v>
+      </c>
+      <c r="P61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62">
+        <f>B56/B57</f>
+        <v>56.668604651162788</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>152</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="0"/>
+        <v>56.668604651162788</v>
+      </c>
+      <c r="P62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63">
         <v>0.8</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C63">
         <v>0.01</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="1">
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>164</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="O63" t="s">
+        <v>161</v>
+      </c>
+      <c r="P63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64">
         <v>0.85</v>
       </c>
-      <c r="C44" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="1">
+      <c r="C64">
+        <v>0.01</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>164</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="O64" t="s">
+        <v>161</v>
+      </c>
+      <c r="P64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65">
         <v>0.9</v>
       </c>
-      <c r="C45" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="1">
-        <v>3500</v>
-      </c>
-      <c r="C46" s="2">
-        <v>150</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="1">
-        <v>3.1999999999999999E-5</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B49" s="1">
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1.4999999999999999E-4</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="C65">
+        <v>0.01</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>164</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="O65" t="s">
+        <v>161</v>
+      </c>
+      <c r="P65" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="1">
-        <v>5.5999999999999999E-5</v>
-      </c>
-      <c r="C52" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="1" t="s">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="C53" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="B66">
+        <v>0.7</v>
+      </c>
+      <c r="C66">
+        <v>0.04</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>167</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="O66" t="s">
+        <v>172</v>
+      </c>
+      <c r="P66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="1">
-        <v>2</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D58" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59">
-        <v>0.97470000000000001</v>
-      </c>
-      <c r="D59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>95</v>
-      </c>
-      <c r="B60">
-        <v>1.72E-2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61">
-        <v>0.4</v>
-      </c>
-      <c r="D61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62">
-        <v>6.8999999999999999E-3</v>
-      </c>
-      <c r="D62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="D63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64">
-        <v>0.98939999999999995</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65">
-        <f>B59/B60</f>
-        <v>56.668604651162788</v>
-      </c>
-      <c r="D65" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>111</v>
-      </c>
-      <c r="B66">
-        <v>0.8</v>
-      </c>
-      <c r="C66">
-        <v>0.01</v>
-      </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>112</v>
-      </c>
-      <c r="B67">
-        <v>0.85</v>
-      </c>
-      <c r="C67">
-        <v>0.01</v>
-      </c>
-      <c r="D67" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>113</v>
-      </c>
-      <c r="B68">
-        <v>0.9</v>
-      </c>
-      <c r="C68">
-        <v>0.01</v>
-      </c>
-      <c r="D68" t="s">
-        <v>5</v>
-      </c>
-      <c r="E68" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>115</v>
-      </c>
-      <c r="B69">
-        <v>0.7</v>
-      </c>
-      <c r="C69">
-        <v>0.04</v>
-      </c>
-      <c r="D69" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" t="s">
-        <v>116</v>
-      </c>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated environmental config and created a combined config
</commit_message>
<xml_diff>
--- a/default_configs/default_environmental_config.xlsx
+++ b/default_configs/default_environmental_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETH\PHD\Manure Tool\default_configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achermann\Project ReFuel\LCA tool developement\Manure Tool\default_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DB62CC-CAF8-412C-BFF6-609512A49B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDC9272-5F6E-410B-B77E-7D0A64D7EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50988" yWindow="-1716" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="183">
   <si>
     <t>value</t>
   </si>
@@ -497,9 +497,6 @@
     <t>lognormal</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -576,6 +573,18 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>factor_field_application_splash_plate</t>
+  </si>
+  <si>
+    <t>factor_field_application_trailing_hose</t>
+  </si>
+  <si>
+    <t>factor_field_application_trailing_shoe</t>
+  </si>
+  <si>
+    <t>stdev95</t>
   </si>
 </sst>
 </file>
@@ -591,7 +600,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,6 +610,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,9 +632,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,23 +917,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7265625" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" customWidth="1"/>
-    <col min="16" max="16" width="84.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="16" max="16" width="23.1796875" customWidth="1"/>
+    <col min="17" max="17" width="84.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -933,40 +950,43 @@
         <v>145</v>
       </c>
       <c r="F1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
         <v>156</v>
       </c>
-      <c r="G1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" t="s">
         <v>157</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>158</v>
       </c>
-      <c r="J1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" t="s">
-        <v>179</v>
-      </c>
       <c r="L1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" t="s">
         <v>176</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>177</v>
       </c>
-      <c r="N1" t="s">
-        <v>178</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>144</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -980,13 +1000,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1000,10 +1020,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1017,10 +1037,10 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1034,13 +1054,13 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
-      </c>
-      <c r="P5" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1054,13 +1074,13 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
-      </c>
-      <c r="P6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1074,13 +1094,13 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
-      </c>
-      <c r="P7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1094,13 +1114,13 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
-      </c>
-      <c r="P8" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1114,13 +1134,13 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
-      </c>
-      <c r="P9" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1134,13 +1154,13 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>154</v>
-      </c>
-      <c r="P10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1154,13 +1174,13 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="P11" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1174,13 +1194,13 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>154</v>
-      </c>
-      <c r="P12" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1194,13 +1214,13 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>154</v>
-      </c>
-      <c r="P13" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1214,13 +1234,13 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
-      </c>
-      <c r="P14" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -1232,10 +1252,10 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>131</v>
       </c>
@@ -1244,10 +1264,10 @@
         <v>0.31818181818181818</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>132</v>
       </c>
@@ -1256,10 +1276,10 @@
         <v>0.82352941176470584</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1272,21 +1292,21 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>153</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:H42" si="0">B18</f>
+        <f t="shared" ref="H18:H45" si="0">B18</f>
         <v>36</v>
       </c>
-      <c r="O18" t="s">
-        <v>173</v>
-      </c>
       <c r="P18" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1299,21 +1319,21 @@
       <c r="D19" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>153</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
         <v>298</v>
       </c>
-      <c r="O19" t="s">
-        <v>173</v>
-      </c>
       <c r="P19" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1326,21 +1346,21 @@
       <c r="D20" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>153</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="O20" t="s">
-        <v>174</v>
-      </c>
       <c r="P20" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -1353,21 +1373,21 @@
       <c r="D21" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>153</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
-      <c r="O21" t="s">
-        <v>167</v>
-      </c>
       <c r="P21" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q21" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -1380,21 +1400,21 @@
       <c r="D22" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>153</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="O22" t="s">
-        <v>167</v>
-      </c>
       <c r="P22" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q22" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -1405,21 +1425,21 @@
       <c r="D23" t="s">
         <v>143</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>153</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
         <v>2.0390277777777778E-2</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>146</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -1430,21 +1450,21 @@
       <c r="D24" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>153</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
         <v>2.8399999999999998E-2</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>147</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -1455,21 +1475,21 @@
       <c r="D25" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>153</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
         <v>36493</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>148</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -1479,21 +1499,21 @@
       <c r="D26" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>153</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
         <v>61.816000000000003</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>149</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -1506,21 +1526,21 @@
       <c r="D27" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>153</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
         <v>44000</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>150</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -1533,21 +1553,21 @@
       <c r="D28" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>153</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>150</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -1560,21 +1580,21 @@
       <c r="D29" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>153</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>150</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -1587,21 +1607,21 @@
       <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>153</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>150</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1627,11 +1647,11 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="O31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1657,11 +1677,11 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="O32" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +1698,7 @@
         <v>151</v>
       </c>
       <c r="F33">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="G33">
         <v>0.8</v>
@@ -1687,14 +1707,14 @@
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
-      <c r="O33" t="s">
-        <v>168</v>
-      </c>
       <c r="P33" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1714,14 +1734,14 @@
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="O34" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="P34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q34" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1736,19 +1756,25 @@
       </c>
       <c r="E35" t="s">
         <v>152</v>
+      </c>
+      <c r="F35">
+        <v>0.58374999999999999</v>
+      </c>
+      <c r="G35">
+        <v>0.35020000000000001</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
         <v>0.46700000000000003</v>
       </c>
-      <c r="O35" t="s">
-        <v>164</v>
-      </c>
       <c r="P35" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1763,24 +1789,30 @@
       </c>
       <c r="E36" t="s">
         <v>152</v>
+      </c>
+      <c r="F36">
+        <v>0.62070000000000003</v>
+      </c>
+      <c r="G36">
+        <v>0.40527000000000002</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
         <v>0.51300000000000001</v>
       </c>
-      <c r="O36" t="s">
-        <v>164</v>
-      </c>
       <c r="P36" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>49</v>
       </c>
       <c r="B37">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="C37">
         <v>0.01</v>
@@ -1791,768 +1823,846 @@
       <c r="E37" t="s">
         <v>152</v>
       </c>
+      <c r="F37">
+        <v>0.53</v>
+      </c>
+      <c r="G37">
+        <v>0.32</v>
+      </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="O37" t="s">
-        <v>164</v>
+        <v>0.43</v>
       </c>
       <c r="P37" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>0.7</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>0.01</v>
       </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="O38" t="s">
-        <v>161</v>
-      </c>
-      <c r="P38" t="s">
+      <c r="P38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39">
-        <v>0.1</v>
-      </c>
-      <c r="C39">
-        <v>0.02</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="E39" t="s">
         <v>152</v>
       </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0.26</v>
+      </c>
       <c r="H39">
+        <v>0.59</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40">
+        <v>0.62</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
+      </c>
+      <c r="H40">
+        <v>0.36</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" s="1">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="O39" t="s">
-        <v>164</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="P42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q42" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>55</v>
       </c>
-      <c r="B40">
+      <c r="B43">
         <v>0.6</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>0.01</v>
       </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
         <v>152</v>
       </c>
-      <c r="H40">
+      <c r="H43">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="B41">
+      <c r="B44">
         <v>0.4</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>0.04</v>
       </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41">
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>59</v>
       </c>
-      <c r="B42">
+      <c r="B45">
         <v>1E-3</v>
       </c>
-      <c r="C42">
+      <c r="C45">
         <v>2E-3</v>
       </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
         <v>152</v>
       </c>
-      <c r="F42">
+      <c r="F45">
         <v>1E-4</v>
       </c>
-      <c r="G42">
+      <c r="G45">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H42">
+      <c r="H45">
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="O42" t="s">
-        <v>165</v>
-      </c>
-      <c r="P42" t="s">
+      <c r="P45" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>61</v>
       </c>
-      <c r="B43">
+      <c r="B46">
         <v>3500</v>
       </c>
-      <c r="C43">
-        <v>150</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C46">
+        <v>1880</v>
+      </c>
+      <c r="D46" t="s">
         <v>62</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E46" t="s">
         <v>152</v>
       </c>
-      <c r="H43">
-        <f t="shared" ref="H43:H66" si="1">B43</f>
+      <c r="H46">
+        <f t="shared" ref="H46:H69" si="1">B46</f>
         <v>3500</v>
       </c>
-      <c r="O43" t="s">
-        <v>164</v>
-      </c>
-      <c r="P43" t="s">
+      <c r="I46">
+        <v>1880</v>
+      </c>
+      <c r="P46" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="B44">
+      <c r="B47">
         <v>0.16</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C47">
+        <v>1.88</v>
+      </c>
+      <c r="D47" t="s">
         <v>62</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E47" t="s">
         <v>152</v>
       </c>
-      <c r="H44">
+      <c r="H47">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="O44" t="s">
-        <v>164</v>
-      </c>
-      <c r="P44" t="s">
+      <c r="I47">
+        <v>1.88</v>
+      </c>
+      <c r="P47" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="48" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B45">
+      <c r="B48" s="1">
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H45">
+      <c r="H48" s="1">
         <f t="shared" si="1"/>
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="O45" t="s">
-        <v>162</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="P48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q48" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="49" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B46">
+      <c r="B49" s="1">
         <v>3.5999999999999998E-6</v>
       </c>
-      <c r="D46" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H46">
+      <c r="H49" s="1">
         <f t="shared" si="1"/>
         <v>3.5999999999999998E-6</v>
       </c>
-      <c r="O46" t="s">
-        <v>162</v>
-      </c>
-      <c r="P46" t="s">
+      <c r="P49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q49" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="50" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B47">
+      <c r="B50" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H47">
+      <c r="H50" s="1">
         <f t="shared" si="1"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="O47" t="s">
-        <v>162</v>
-      </c>
-      <c r="P47" t="s">
+      <c r="P50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="51" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B48">
+      <c r="B51" s="1">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="D48" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H48">
+      <c r="H51" s="1">
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="O48" t="s">
-        <v>162</v>
-      </c>
-      <c r="P48" t="s">
+      <c r="P51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q51" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B49">
+      <c r="B52" s="1">
         <v>5.5999999999999999E-5</v>
       </c>
-      <c r="C49">
+      <c r="C52" s="1">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="D49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H49">
+      <c r="H52" s="1">
         <f t="shared" si="1"/>
         <v>5.5999999999999999E-5</v>
       </c>
-      <c r="O49" t="s">
-        <v>162</v>
-      </c>
-      <c r="P49" t="s">
+      <c r="P52" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q52" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="53" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B50">
+      <c r="B53" s="1">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="C50">
+      <c r="C53" s="1">
         <v>1E-4</v>
       </c>
-      <c r="D50" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H50">
+      <c r="H53" s="1">
         <f t="shared" si="1"/>
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="O50" t="s">
-        <v>162</v>
-      </c>
-      <c r="P50" t="s">
+      <c r="P53" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q53" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>93</v>
       </c>
-      <c r="B51">
+      <c r="B54">
         <v>1.5</v>
       </c>
-      <c r="D51" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
         <v>151</v>
       </c>
-      <c r="F51">
+      <c r="F54">
         <v>4</v>
       </c>
-      <c r="G51">
+      <c r="G54">
         <v>1.2</v>
       </c>
-      <c r="H51">
+      <c r="H54">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="O51" t="s">
-        <v>169</v>
-      </c>
-      <c r="P51" t="s">
+      <c r="P54" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q54" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>95</v>
       </c>
-      <c r="B52">
+      <c r="B55">
         <v>0.5</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D55" t="s">
         <v>96</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E55" t="s">
         <v>152</v>
       </c>
-      <c r="F52">
+      <c r="F55">
         <v>0.6</v>
       </c>
-      <c r="G52">
+      <c r="G55">
         <v>0.2</v>
       </c>
-      <c r="H52">
+      <c r="H55">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="O52" t="s">
-        <v>175</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="P55" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>72</v>
       </c>
-      <c r="B53">
+      <c r="B56">
         <v>0.7</v>
       </c>
-      <c r="D53" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H53">
+      <c r="D56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="O53" t="s">
-        <v>170</v>
-      </c>
-      <c r="P53" t="s">
+      <c r="P56" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q56" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>84</v>
       </c>
-      <c r="B54">
+      <c r="B57">
         <v>0.3</v>
       </c>
-      <c r="D54" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H54">
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H57">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="O54" t="s">
-        <v>170</v>
-      </c>
-      <c r="P54" t="s">
+      <c r="P57" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="58" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B55">
+      <c r="B58" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E58" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H55">
+      <c r="H58" s="1">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="O55" t="s">
-        <v>172</v>
-      </c>
-      <c r="P55" t="s">
+      <c r="P58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q58" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="59" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B56">
+      <c r="B59" s="1">
         <v>0.97470000000000001</v>
       </c>
-      <c r="D56" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H56">
+      <c r="H59" s="1">
         <f t="shared" si="1"/>
         <v>0.97470000000000001</v>
       </c>
-      <c r="O56" t="s">
-        <v>170</v>
-      </c>
-      <c r="P56" t="s">
+      <c r="P59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q59" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B57">
+      <c r="B60" s="1">
         <v>1.72E-2</v>
       </c>
-      <c r="D57" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="D60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H57">
+      <c r="H60" s="1">
         <f t="shared" si="1"/>
         <v>1.72E-2</v>
       </c>
-      <c r="O57" t="s">
-        <v>172</v>
-      </c>
-      <c r="P57" t="s">
+      <c r="P60" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q60" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="61" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B58">
+      <c r="B61" s="1">
         <v>0.4</v>
       </c>
-      <c r="D58" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H58">
+      <c r="H61" s="1">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="O58" t="s">
-        <v>172</v>
-      </c>
-      <c r="P58" t="s">
+      <c r="P61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q61" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B59">
+      <c r="B62" s="1">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="D59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H59">
+      <c r="H62" s="1">
         <f t="shared" si="1"/>
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="O59" t="s">
-        <v>172</v>
-      </c>
-      <c r="P59" t="s">
+      <c r="P62" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q62" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="63" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B60">
+      <c r="B63" s="1">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="D60" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H60">
+      <c r="H63" s="1">
         <f t="shared" si="1"/>
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="O60" t="s">
-        <v>172</v>
-      </c>
-      <c r="P60" t="s">
+      <c r="P63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q63" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="64" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B61">
+      <c r="B64" s="1">
         <v>0.98939999999999995</v>
       </c>
-      <c r="D61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H61">
+      <c r="H64" s="1">
         <f t="shared" si="1"/>
         <v>0.98939999999999995</v>
       </c>
-      <c r="O61" t="s">
-        <v>172</v>
-      </c>
-      <c r="P61" t="s">
+      <c r="P64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q64" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="65" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B62">
-        <f>B56/B57</f>
+      <c r="B65" s="1">
+        <f>B59/B60</f>
         <v>56.668604651162788</v>
       </c>
-      <c r="D62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="D65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H62">
+      <c r="H65" s="1">
         <f t="shared" si="1"/>
         <v>56.668604651162788</v>
       </c>
-      <c r="P62" t="s">
+      <c r="Q65" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>105</v>
       </c>
-      <c r="B63">
+      <c r="B66">
         <v>0.8</v>
       </c>
-      <c r="C63">
+      <c r="C66">
         <v>0.01</v>
       </c>
-      <c r="D63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" t="s">
-        <v>163</v>
-      </c>
-      <c r="F63">
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F66">
         <v>0.85</v>
       </c>
-      <c r="G63">
+      <c r="G66">
         <v>0.75</v>
       </c>
-      <c r="H63">
+      <c r="H66">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="O63" t="s">
-        <v>160</v>
-      </c>
-      <c r="P63" t="s">
+      <c r="P66" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q66" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>106</v>
       </c>
-      <c r="B64">
+      <c r="B67">
         <v>0.85</v>
       </c>
-      <c r="C64">
+      <c r="C67">
         <v>0.01</v>
       </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" t="s">
-        <v>163</v>
-      </c>
-      <c r="F64">
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>162</v>
+      </c>
+      <c r="F67">
         <v>0.9</v>
       </c>
-      <c r="G64">
+      <c r="G67">
         <v>0.8</v>
       </c>
-      <c r="H64">
+      <c r="H67">
         <f t="shared" si="1"/>
         <v>0.85</v>
       </c>
-      <c r="O64" t="s">
-        <v>160</v>
-      </c>
-      <c r="P64" t="s">
+      <c r="P67" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q67" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>107</v>
       </c>
-      <c r="B65">
+      <c r="B68">
         <v>0.9</v>
       </c>
-      <c r="C65">
+      <c r="C68">
         <v>0.01</v>
       </c>
-      <c r="D65" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" t="s">
-        <v>163</v>
-      </c>
-      <c r="F65">
+      <c r="D68" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>162</v>
+      </c>
+      <c r="F68">
         <v>0.95</v>
       </c>
-      <c r="G65">
+      <c r="G68">
         <v>0.85</v>
       </c>
-      <c r="H65">
+      <c r="H68">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="O65" t="s">
-        <v>160</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="P68" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q68" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>109</v>
       </c>
-      <c r="B66">
+      <c r="B69">
         <v>0.7</v>
       </c>
-      <c r="C66">
+      <c r="C69">
         <v>0.04</v>
       </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" t="s">
-        <v>166</v>
-      </c>
-      <c r="H66">
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>165</v>
+      </c>
+      <c r="F69">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G69">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="H69">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="O66" t="s">
-        <v>171</v>
-      </c>
-      <c r="P66" t="s">
+      <c r="P69" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q69" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>